<commit_message>
Update to new SS version 3.30.18
</commit_message>
<xml_diff>
--- a/Example data files/Life history.xlsx
+++ b/Example data files/Life history.xlsx
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update life history file to fix priors
</commit_message>
<xml_diff>
--- a/Example data files/Life history.xlsx
+++ b/Example data files/Life history.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Cope\Documents\Github\SS-DL-tool\Example data files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\copej\Documents\GitHub\SS-DL-tool\Example data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1206D-7BB6-4208-88DD-E0066E5D9472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Female</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t>Linf</t>
-  </si>
-  <si>
-    <t>Normal</t>
   </si>
   <si>
     <t>k</t>
@@ -131,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,28 +479,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,10 +514,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -536,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -547,15 +545,15 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>0.12770000000000001</v>
@@ -564,15 +562,15 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>-2.4390000000000001</v>
@@ -581,32 +579,32 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>39.4</v>
@@ -615,9 +613,9 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>48</v>
@@ -626,20 +624,20 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>2.9273210000000001</v>
@@ -648,9 +646,9 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3">
         <v>4.32E-7</v>
@@ -659,9 +657,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3">
         <v>3.548</v>
@@ -670,16 +668,16 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -696,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -707,15 +705,15 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="3">
         <v>0.14849999999999999</v>
@@ -724,15 +722,15 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="3">
         <v>-1.952</v>
@@ -741,43 +739,43 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2">
         <v>0.1</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2">
         <v>2.8293140000000001</v>
@@ -786,46 +784,46 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>